<commit_message>
JAMP - added debugging and changed parameter for maxResults
</commit_message>
<xml_diff>
--- a/pandas_simple.xlsx
+++ b/pandas_simple.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="38">
   <si>
     <t>Team</t>
   </si>
@@ -62,6 +62,18 @@
   </si>
   <si>
     <t>JAMP board</t>
+  </si>
+  <si>
+    <t>JAMP Team 2</t>
+  </si>
+  <si>
+    <t>JAMP Team 3</t>
+  </si>
+  <si>
+    <t>JAMP Team 4</t>
+  </si>
+  <si>
+    <t>JAMP Team 1</t>
   </si>
   <si>
     <t>Sprint 1.1</t>
@@ -473,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -534,7 +546,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>11</v>
@@ -581,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -622,7 +634,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -657,7 +669,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -689,7 +701,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -721,7 +733,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -753,7 +765,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -785,7 +797,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -817,7 +829,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -849,7 +861,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -881,7 +893,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -913,7 +925,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -945,7 +957,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -977,7 +989,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1009,7 +1021,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1041,7 +1053,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1073,7 +1085,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1105,7 +1117,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1130,6 +1142,1484 @@
       </c>
       <c r="P19">
         <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>34</v>
+      </c>
+      <c r="K20">
+        <v>8</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>8</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>25</v>
+      </c>
+      <c r="K21">
+        <v>7</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>7</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>11</v>
+      </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>6</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>35</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>10</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>25</v>
+      </c>
+      <c r="K24">
+        <v>6</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>6</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>27</v>
+      </c>
+      <c r="K25">
+        <v>10</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>10</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>27</v>
+      </c>
+      <c r="K26">
+        <v>7</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>7</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>15</v>
+      </c>
+      <c r="K27">
+        <v>5</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>5</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>44</v>
+      </c>
+      <c r="K28">
+        <v>10</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>10</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>22</v>
+      </c>
+      <c r="K29">
+        <v>6</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>6</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>24</v>
+      </c>
+      <c r="K30">
+        <v>7</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>7</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>32</v>
+      </c>
+      <c r="K31">
+        <v>8</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>8</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>38</v>
+      </c>
+      <c r="K32">
+        <v>10</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>10</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>13</v>
+      </c>
+      <c r="K33">
+        <v>5</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>5</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>18</v>
+      </c>
+      <c r="K34">
+        <v>6</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>6</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>32</v>
+      </c>
+      <c r="K35">
+        <v>8</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>8</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>36</v>
+      </c>
+      <c r="K36">
+        <v>8</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>8</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>12</v>
+      </c>
+      <c r="K37">
+        <v>5</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>5</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>25</v>
+      </c>
+      <c r="K38">
+        <v>5</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>5</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>18</v>
+      </c>
+      <c r="K39">
+        <v>5</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>5</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>13</v>
+      </c>
+      <c r="K40">
+        <v>6</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>6</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>38</v>
+      </c>
+      <c r="K41">
+        <v>10</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>10</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>37</v>
+      </c>
+      <c r="K42">
+        <v>7</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>7</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>37</v>
+      </c>
+      <c r="K43">
+        <v>8</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>8</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>27</v>
+      </c>
+      <c r="K44">
+        <v>8</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>8</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>31</v>
+      </c>
+      <c r="K45">
+        <v>7</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>7</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>40</v>
+      </c>
+      <c r="K46">
+        <v>9</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>9</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>19</v>
+      </c>
+      <c r="K47">
+        <v>5</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>5</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>43</v>
+      </c>
+      <c r="K48">
+        <v>10</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>10</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>44</v>
+      </c>
+      <c r="K49">
+        <v>10</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>10</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>24</v>
+      </c>
+      <c r="K50">
+        <v>5</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>5</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>38</v>
+      </c>
+      <c r="K51">
+        <v>9</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>9</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>40</v>
+      </c>
+      <c r="K52">
+        <v>10</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>10</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>30</v>
+      </c>
+      <c r="K53">
+        <v>5</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>5</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>23</v>
+      </c>
+      <c r="K54">
+        <v>5</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>5</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>18</v>
+      </c>
+      <c r="K55">
+        <v>5</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>5</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" t="s">
+        <v>29</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>18</v>
+      </c>
+      <c r="K56">
+        <v>7</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>7</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" t="s">
+        <v>30</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>46</v>
+      </c>
+      <c r="K57">
+        <v>10</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>10</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>18</v>
+      </c>
+      <c r="K58">
+        <v>6</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>6</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>32</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>43</v>
+      </c>
+      <c r="K59">
+        <v>10</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>10</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>27</v>
+      </c>
+      <c r="K60">
+        <v>7</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>7</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>44</v>
+      </c>
+      <c r="K61">
+        <v>8</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>8</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>29</v>
+      </c>
+      <c r="K62">
+        <v>7</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>7</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" t="s">
+        <v>36</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>27</v>
+      </c>
+      <c r="K63">
+        <v>8</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>8</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" t="s">
+        <v>37</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>26</v>
+      </c>
+      <c r="K64">
+        <v>5</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>5</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>5</v>
+      </c>
+      <c r="H65">
+        <v>5</v>
+      </c>
+      <c r="I65">
+        <v>5</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>1</v>
+      </c>
+      <c r="P65">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Windows 64 Bit build based on latest submitted baseline.
</commit_message>
<xml_diff>
--- a/pandas_simple.xlsx
+++ b/pandas_simple.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="35">
   <si>
     <t>Team</t>
   </si>
@@ -61,9 +61,6 @@
     <t># Issues Completed</t>
   </si>
   <si>
-    <t>JAMP board</t>
-  </si>
-  <si>
     <t>JAMP Team 2</t>
   </si>
   <si>
@@ -76,58 +73,52 @@
     <t>JAMP Team 1</t>
   </si>
   <si>
+    <t>API-JAMP Sprint 1.1</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 1.2</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 1.3</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 1.4</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 1.5</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 2.1</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 2.2</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 2.3</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 2.4</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 2.5</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 3.1</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 3.2</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 3.3</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 3.4</t>
+  </si>
+  <si>
+    <t>API-JAMP Sprint 3.5</t>
+  </si>
+  <si>
     <t>Sprint 1.1</t>
-  </si>
-  <si>
-    <t>Sprint 1.2</t>
-  </si>
-  <si>
-    <t>Sprint 1.3</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 1.1</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 1.2</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 1.3</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 1.4</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 1.5</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 2.1</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 2.2</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 2.3</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 2.4</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 2.5</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 3.1</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 3.2</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 3.3</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 3.4</t>
-  </si>
-  <si>
-    <t>API-JAMP Sprint 3.5</t>
   </si>
 </sst>
 </file>
@@ -485,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -546,46 +537,31 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G2">
+        <v>34</v>
+      </c>
+      <c r="K2">
         <v>8</v>
       </c>
-      <c r="H2">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>8</v>
       </c>
-      <c r="I2">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>0.7272727272727273</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
       <c r="O2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -593,40 +569,31 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>16</v>
-      </c>
-      <c r="I3">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="K3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -634,28 +601,25 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="K4">
         <v>6</v>
       </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
       <c r="L4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -669,16 +633,16 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="K5">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -687,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -701,16 +665,16 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="K6">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -719,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -733,16 +697,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="K7">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -751,7 +715,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -765,16 +729,16 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="K8">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -783,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -797,16 +761,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="K9">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -815,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -829,16 +793,16 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="K10">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -847,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -861,16 +825,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="K11">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -879,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -893,16 +857,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="K12">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -911,7 +875,7 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -925,16 +889,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="K13">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -943,7 +907,7 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -957,16 +921,16 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="K14">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -975,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -989,16 +953,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="G15">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="K15">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1007,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -1021,16 +985,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="K16">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -1039,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -1050,19 +1014,19 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="K17">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1071,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1082,19 +1046,19 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="G18">
         <v>36</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>83</v>
-      </c>
       <c r="K18">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1103,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="N18">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1114,19 +1078,19 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="K19">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1135,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="N19">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1149,16 +1113,16 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="K20">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -1167,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1181,16 +1145,16 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="G21">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="K21">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -1199,7 +1163,7 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1213,13 +1177,13 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="G22">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K22">
         <v>6</v>
@@ -1245,13 +1209,13 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K23">
         <v>10</v>
@@ -1277,16 +1241,16 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="K24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -1295,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1309,16 +1273,16 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="K25">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -1327,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1341,7 +1305,7 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1350,7 +1314,7 @@
         <v>27</v>
       </c>
       <c r="K26">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -1359,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="N26">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1373,16 +1337,16 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="K27">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -1391,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="N27">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -1405,16 +1369,16 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -1423,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O28">
         <v>0</v>
@@ -1437,16 +1401,16 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="G29">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K29">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -1455,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O29">
         <v>0</v>
@@ -1469,16 +1433,16 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="G30">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="K30">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -1487,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="N30">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O30">
         <v>0</v>
@@ -1501,16 +1465,16 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="G31">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="K31">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -1519,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="N31">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O31">
         <v>0</v>
@@ -1530,19 +1494,19 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="G32">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="K32">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -1551,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="N32">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O32">
         <v>0</v>
@@ -1562,19 +1526,19 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="G33">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="K33">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -1583,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="N33">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O33">
         <v>0</v>
@@ -1594,19 +1558,19 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="G34">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="K34">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -1615,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="N34">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O34">
         <v>0</v>
@@ -1629,16 +1593,16 @@
         <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="G35">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K35">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -1647,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O35">
         <v>0</v>
@@ -1661,16 +1625,16 @@
         <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="G36">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="K36">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -1679,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="N36">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -1693,13 +1657,13 @@
         <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="G37">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="K37">
         <v>5</v>
@@ -1725,16 +1689,16 @@
         <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="G38">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="K38">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L38">
         <v>0</v>
@@ -1743,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O38">
         <v>0</v>
@@ -1757,16 +1721,16 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="G39">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="K39">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L39">
         <v>0</v>
@@ -1775,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O39">
         <v>0</v>
@@ -1789,13 +1753,13 @@
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="G40">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="K40">
         <v>6</v>
@@ -1821,13 +1785,13 @@
         <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="G41">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="K41">
         <v>10</v>
@@ -1853,13 +1817,13 @@
         <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="G42">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="K42">
         <v>7</v>
@@ -1885,13 +1849,13 @@
         <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="K43">
         <v>8</v>
@@ -1917,16 +1881,16 @@
         <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="G44">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K44">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L44">
         <v>0</v>
@@ -1935,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="N44">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O44">
         <v>0</v>
@@ -1949,16 +1913,16 @@
         <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="G45">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L45">
         <v>0</v>
@@ -1967,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="N45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O45">
         <v>0</v>
@@ -1981,16 +1945,16 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="G46">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="K46">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L46">
         <v>0</v>
@@ -1999,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="N46">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -2010,615 +1974,39 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="I47">
+        <v>5</v>
       </c>
       <c r="K47">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47">
         <v>0</v>
       </c>
       <c r="N47">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="A48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>43</v>
-      </c>
-      <c r="K48">
-        <v>10</v>
-      </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-      <c r="M48">
-        <v>0</v>
-      </c>
-      <c r="N48">
-        <v>10</v>
-      </c>
-      <c r="O48">
-        <v>0</v>
-      </c>
-      <c r="P48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16">
-      <c r="A49" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" t="s">
-        <v>37</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <v>44</v>
-      </c>
-      <c r="K49">
-        <v>10</v>
-      </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49">
-        <v>0</v>
-      </c>
-      <c r="N49">
-        <v>10</v>
-      </c>
-      <c r="O49">
-        <v>0</v>
-      </c>
-      <c r="P49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16">
-      <c r="A50" t="s">
-        <v>18</v>
-      </c>
-      <c r="B50" t="s">
-        <v>23</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>24</v>
-      </c>
-      <c r="K50">
-        <v>5</v>
-      </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-      <c r="M50">
-        <v>0</v>
-      </c>
-      <c r="N50">
-        <v>5</v>
-      </c>
-      <c r="O50">
-        <v>0</v>
-      </c>
-      <c r="P50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16">
-      <c r="A51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" t="s">
-        <v>24</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <v>38</v>
-      </c>
-      <c r="K51">
-        <v>9</v>
-      </c>
-      <c r="L51">
-        <v>0</v>
-      </c>
-      <c r="M51">
-        <v>0</v>
-      </c>
-      <c r="N51">
-        <v>9</v>
-      </c>
-      <c r="O51">
-        <v>0</v>
-      </c>
-      <c r="P51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16">
-      <c r="A52" t="s">
-        <v>18</v>
-      </c>
-      <c r="B52" t="s">
-        <v>25</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>40</v>
-      </c>
-      <c r="K52">
-        <v>10</v>
-      </c>
-      <c r="L52">
-        <v>0</v>
-      </c>
-      <c r="M52">
-        <v>0</v>
-      </c>
-      <c r="N52">
-        <v>10</v>
-      </c>
-      <c r="O52">
-        <v>0</v>
-      </c>
-      <c r="P52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16">
-      <c r="A53" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" t="s">
-        <v>26</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="G53">
-        <v>30</v>
-      </c>
-      <c r="K53">
-        <v>5</v>
-      </c>
-      <c r="L53">
-        <v>0</v>
-      </c>
-      <c r="M53">
-        <v>0</v>
-      </c>
-      <c r="N53">
-        <v>5</v>
-      </c>
-      <c r="O53">
-        <v>0</v>
-      </c>
-      <c r="P53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16">
-      <c r="A54" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="G54">
-        <v>23</v>
-      </c>
-      <c r="K54">
-        <v>5</v>
-      </c>
-      <c r="L54">
-        <v>0</v>
-      </c>
-      <c r="M54">
-        <v>0</v>
-      </c>
-      <c r="N54">
-        <v>5</v>
-      </c>
-      <c r="O54">
-        <v>0</v>
-      </c>
-      <c r="P54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16">
-      <c r="A55" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55" t="s">
-        <v>28</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>18</v>
-      </c>
-      <c r="K55">
-        <v>5</v>
-      </c>
-      <c r="L55">
-        <v>0</v>
-      </c>
-      <c r="M55">
-        <v>0</v>
-      </c>
-      <c r="N55">
-        <v>5</v>
-      </c>
-      <c r="O55">
-        <v>0</v>
-      </c>
-      <c r="P55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16">
-      <c r="A56" t="s">
-        <v>18</v>
-      </c>
-      <c r="B56" t="s">
-        <v>29</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>18</v>
-      </c>
-      <c r="K56">
-        <v>7</v>
-      </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-      <c r="M56">
-        <v>0</v>
-      </c>
-      <c r="N56">
-        <v>7</v>
-      </c>
-      <c r="O56">
-        <v>0</v>
-      </c>
-      <c r="P56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16">
-      <c r="A57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" t="s">
-        <v>30</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="G57">
-        <v>46</v>
-      </c>
-      <c r="K57">
-        <v>10</v>
-      </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-      <c r="M57">
-        <v>0</v>
-      </c>
-      <c r="N57">
-        <v>10</v>
-      </c>
-      <c r="O57">
-        <v>0</v>
-      </c>
-      <c r="P57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16">
-      <c r="A58" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="G58">
-        <v>18</v>
-      </c>
-      <c r="K58">
-        <v>6</v>
-      </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-      <c r="M58">
-        <v>0</v>
-      </c>
-      <c r="N58">
-        <v>6</v>
-      </c>
-      <c r="O58">
-        <v>0</v>
-      </c>
-      <c r="P58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16">
-      <c r="A59" t="s">
-        <v>18</v>
-      </c>
-      <c r="B59" t="s">
-        <v>32</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="G59">
-        <v>43</v>
-      </c>
-      <c r="K59">
-        <v>10</v>
-      </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-      <c r="M59">
-        <v>0</v>
-      </c>
-      <c r="N59">
-        <v>10</v>
-      </c>
-      <c r="O59">
-        <v>0</v>
-      </c>
-      <c r="P59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16">
-      <c r="A60" t="s">
-        <v>18</v>
-      </c>
-      <c r="B60" t="s">
-        <v>33</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="G60">
-        <v>27</v>
-      </c>
-      <c r="K60">
-        <v>7</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-      <c r="M60">
-        <v>0</v>
-      </c>
-      <c r="N60">
-        <v>7</v>
-      </c>
-      <c r="O60">
-        <v>0</v>
-      </c>
-      <c r="P60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16">
-      <c r="A61" t="s">
-        <v>18</v>
-      </c>
-      <c r="B61" t="s">
-        <v>34</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="G61">
-        <v>44</v>
-      </c>
-      <c r="K61">
-        <v>8</v>
-      </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-      <c r="M61">
-        <v>0</v>
-      </c>
-      <c r="N61">
-        <v>8</v>
-      </c>
-      <c r="O61">
-        <v>0</v>
-      </c>
-      <c r="P61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16">
-      <c r="A62" t="s">
-        <v>18</v>
-      </c>
-      <c r="B62" t="s">
-        <v>35</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="G62">
-        <v>29</v>
-      </c>
-      <c r="K62">
-        <v>7</v>
-      </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-      <c r="M62">
-        <v>0</v>
-      </c>
-      <c r="N62">
-        <v>7</v>
-      </c>
-      <c r="O62">
-        <v>0</v>
-      </c>
-      <c r="P62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16">
-      <c r="A63" t="s">
-        <v>18</v>
-      </c>
-      <c r="B63" t="s">
-        <v>36</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="G63">
-        <v>27</v>
-      </c>
-      <c r="K63">
-        <v>8</v>
-      </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
-      <c r="M63">
-        <v>0</v>
-      </c>
-      <c r="N63">
-        <v>8</v>
-      </c>
-      <c r="O63">
-        <v>0</v>
-      </c>
-      <c r="P63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16">
-      <c r="A64" t="s">
-        <v>18</v>
-      </c>
-      <c r="B64" t="s">
-        <v>37</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="G64">
-        <v>26</v>
-      </c>
-      <c r="K64">
-        <v>5</v>
-      </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
-      <c r="M64">
-        <v>0</v>
-      </c>
-      <c r="N64">
-        <v>5</v>
-      </c>
-      <c r="O64">
-        <v>0</v>
-      </c>
-      <c r="P64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16">
-      <c r="A65" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" t="s">
-        <v>20</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>5</v>
-      </c>
-      <c r="H65">
-        <v>5</v>
-      </c>
-      <c r="I65">
-        <v>5</v>
-      </c>
-      <c r="K65">
-        <v>1</v>
-      </c>
-      <c r="L65">
-        <v>1</v>
-      </c>
-      <c r="M65">
-        <v>0</v>
-      </c>
-      <c r="N65">
-        <v>0</v>
-      </c>
-      <c r="O65">
-        <v>1</v>
-      </c>
-      <c r="P65">
         <v>1</v>
       </c>
     </row>

</xml_diff>